<commit_message>
Fixed custom field settings bug for leaf nodes.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableCustomColumnFieldSubtotals.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableCustomColumnFieldSubtotals.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03618A89-2304-43E8-80F8-B47C068FD003}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24390" windowHeight="10530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24396" windowHeight="10536" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="40">
   <si>
     <t>Transaction</t>
   </si>
@@ -136,12 +137,24 @@
   </si>
   <si>
     <t>Tent Product</t>
+  </si>
+  <si>
+    <t>Chicago Total</t>
+  </si>
+  <si>
+    <t>Nashville Total</t>
+  </si>
+  <si>
+    <t>San Francisco Total</t>
+  </si>
+  <si>
+    <t>Sum of Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -247,7 +260,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Evan M. Schallerer" refreshedDate="43497.544572800929" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="7">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Evan M. Schallerer" refreshedDate="43497.544572800929" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="7" xr:uid="{00000000-000A-0000-FFFF-FFFF04000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B2:H9" sheet="Sheet1"/>
   </cacheSource>
@@ -302,7 +315,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="7">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="7">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -370,7 +383,131 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E84011C2-03FC-4024-823E-C45B7B55DC36}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F47:V53" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" countASubtotal="1" maxSubtotal="1" minSubtotal="1">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="countA"/>
+        <item t="max"/>
+        <item t="min"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </colFields>
+  <colItems count="16">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="countA">
+      <x v="1048832"/>
+      <x/>
+    </i>
+    <i t="max" r="1">
+      <x/>
+    </i>
+    <i t="min" r="1">
+      <x/>
+    </i>
+    <i t="countA" r="1">
+      <x v="1"/>
+    </i>
+    <i t="max" r="1">
+      <x v="1"/>
+    </i>
+    <i t="min" r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable3" cacheId="1" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F16:Q42" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
@@ -542,12 +679,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F3:U7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -654,12 +794,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F10:Q13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -735,6 +878,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -1002,17 +1148,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>20100076</v>
       </c>
@@ -1058,7 +1204,7 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>20100085</v>
       </c>
@@ -1081,7 +1227,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>20100083</v>
       </c>
@@ -1104,7 +1250,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>20100007</v>
       </c>
@@ -1127,7 +1273,7 @@
         <v>831.5</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>20100070</v>
       </c>
@@ -1150,7 +1296,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>20100017</v>
       </c>
@@ -1173,7 +1319,7 @@
         <v>831.5</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>20100090</v>
       </c>
@@ -1202,42 +1348,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F3:U42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="F3:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
-    <col min="14" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="18" width="9" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" customWidth="1"/>
-    <col min="20" max="21" width="11.28515625" customWidth="1"/>
-    <col min="22" max="22" width="35" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:21" x14ac:dyDescent="0.3">
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:21" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>8</v>
       </c>
@@ -1272,7 +1422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1295,7 +1445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1345,7 +1495,7 @@
         <v>1985.99</v>
       </c>
     </row>
-    <row r="7" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1395,12 +1545,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:21" x14ac:dyDescent="0.3">
       <c r="G10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:21" x14ac:dyDescent="0.3">
       <c r="G11" t="s">
         <v>8</v>
       </c>
@@ -1423,7 +1573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:21" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
         <v>12</v>
       </c>
@@ -1443,7 +1593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>16</v>
       </c>
@@ -1481,12 +1631,12 @@
         <v>1985.99</v>
       </c>
     </row>
-    <row r="16" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:21" x14ac:dyDescent="0.3">
       <c r="G16" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:17" x14ac:dyDescent="0.3">
       <c r="G17" t="s">
         <v>9</v>
       </c>
@@ -1509,7 +1659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F18" s="3" t="s">
         <v>30</v>
       </c>
@@ -1535,7 +1685,7 @@
         <v>20100083</v>
       </c>
     </row>
-    <row r="19" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1551,7 +1701,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F20" s="6" t="s">
         <v>8</v>
       </c>
@@ -1567,7 +1717,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F21" s="7" t="s">
         <v>12</v>
       </c>
@@ -1589,7 +1739,7 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="22" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F22" s="7" t="s">
         <v>14</v>
       </c>
@@ -1613,7 +1763,7 @@
         <v>831.5</v>
       </c>
     </row>
-    <row r="23" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F23" s="7" t="s">
         <v>7</v>
       </c>
@@ -1635,7 +1785,7 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="24" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F24" s="6" t="s">
         <v>19</v>
       </c>
@@ -1661,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F25" s="6" t="s">
         <v>10</v>
       </c>
@@ -1677,7 +1827,7 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F26" s="7" t="s">
         <v>12</v>
       </c>
@@ -1699,7 +1849,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="27" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F27" s="7" t="s">
         <v>14</v>
       </c>
@@ -1721,7 +1871,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F28" s="7" t="s">
         <v>7</v>
       </c>
@@ -1743,7 +1893,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F29" s="6" t="s">
         <v>23</v>
       </c>
@@ -1767,7 +1917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F30" s="4" t="s">
         <v>17</v>
       </c>
@@ -1783,7 +1933,7 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F31" s="6" t="s">
         <v>8</v>
       </c>
@@ -1799,7 +1949,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F32" s="7" t="s">
         <v>12</v>
       </c>
@@ -1821,7 +1971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F33" s="7" t="s">
         <v>14</v>
       </c>
@@ -1845,7 +1995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F34" s="7" t="s">
         <v>7</v>
       </c>
@@ -1867,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F35" s="6" t="s">
         <v>19</v>
       </c>
@@ -1893,7 +2043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F36" s="6" t="s">
         <v>10</v>
       </c>
@@ -1909,7 +2059,7 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F37" s="7" t="s">
         <v>12</v>
       </c>
@@ -1931,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F38" s="7" t="s">
         <v>14</v>
       </c>
@@ -1953,7 +2103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F39" s="7" t="s">
         <v>7</v>
       </c>
@@ -1975,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F40" s="6" t="s">
         <v>23</v>
       </c>
@@ -1999,7 +2149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F41" s="4" t="s">
         <v>31</v>
       </c>
@@ -2037,7 +2187,7 @@
         <v>1985.99</v>
       </c>
     </row>
-    <row r="42" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:22" x14ac:dyDescent="0.3">
       <c r="F42" s="4" t="s">
         <v>32</v>
       </c>
@@ -2073,6 +2223,242 @@
       </c>
       <c r="Q42" s="5">
         <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="6:22" x14ac:dyDescent="0.3">
+      <c r="F47" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="6:22" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" t="s">
+        <v>36</v>
+      </c>
+      <c r="J48" t="s">
+        <v>14</v>
+      </c>
+      <c r="L48" t="s">
+        <v>37</v>
+      </c>
+      <c r="M48" t="s">
+        <v>7</v>
+      </c>
+      <c r="O48" t="s">
+        <v>38</v>
+      </c>
+      <c r="V48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="6:22" x14ac:dyDescent="0.3">
+      <c r="F49" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" t="s">
+        <v>10</v>
+      </c>
+      <c r="J49" t="s">
+        <v>8</v>
+      </c>
+      <c r="K49" t="s">
+        <v>10</v>
+      </c>
+      <c r="M49" t="s">
+        <v>8</v>
+      </c>
+      <c r="N49" t="s">
+        <v>10</v>
+      </c>
+      <c r="P49" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>21</v>
+      </c>
+      <c r="R49" t="s">
+        <v>28</v>
+      </c>
+      <c r="S49" t="s">
+        <v>23</v>
+      </c>
+      <c r="T49" t="s">
+        <v>25</v>
+      </c>
+      <c r="U49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="6:22" x14ac:dyDescent="0.3">
+      <c r="F50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="5">
+        <v>831.5</v>
+      </c>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5">
+        <v>831.5</v>
+      </c>
+      <c r="J50" s="5">
+        <v>1663</v>
+      </c>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5">
+        <v>1663</v>
+      </c>
+      <c r="M50" s="5">
+        <v>415.75</v>
+      </c>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5">
+        <v>415.75</v>
+      </c>
+      <c r="P50" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q50" s="5">
+        <v>831.5</v>
+      </c>
+      <c r="R50" s="5">
+        <v>415.75</v>
+      </c>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5">
+        <v>2910.25</v>
+      </c>
+    </row>
+    <row r="51" spans="6:22" x14ac:dyDescent="0.3">
+      <c r="F51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5">
+        <v>99</v>
+      </c>
+      <c r="O51" s="5">
+        <v>99</v>
+      </c>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5">
+        <v>1</v>
+      </c>
+      <c r="T51" s="5">
+        <v>99</v>
+      </c>
+      <c r="U51" s="5">
+        <v>99</v>
+      </c>
+      <c r="V51" s="5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="6:22" x14ac:dyDescent="0.3">
+      <c r="F52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5">
+        <v>24.99</v>
+      </c>
+      <c r="I52" s="5">
+        <v>24.99</v>
+      </c>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5">
+        <v>1194</v>
+      </c>
+      <c r="L52" s="5">
+        <v>1194</v>
+      </c>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5">
+        <v>2</v>
+      </c>
+      <c r="T52" s="5">
+        <v>1194</v>
+      </c>
+      <c r="U52" s="5">
+        <v>24.99</v>
+      </c>
+      <c r="V52" s="5">
+        <v>1218.99</v>
+      </c>
+    </row>
+    <row r="53" spans="6:22" x14ac:dyDescent="0.3">
+      <c r="F53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="5">
+        <v>831.5</v>
+      </c>
+      <c r="H53" s="5">
+        <v>24.99</v>
+      </c>
+      <c r="I53" s="5">
+        <v>856.49</v>
+      </c>
+      <c r="J53" s="5">
+        <v>1663</v>
+      </c>
+      <c r="K53" s="5">
+        <v>1194</v>
+      </c>
+      <c r="L53" s="5">
+        <v>2857</v>
+      </c>
+      <c r="M53" s="5">
+        <v>415.75</v>
+      </c>
+      <c r="N53" s="5">
+        <v>99</v>
+      </c>
+      <c r="O53" s="5">
+        <v>514.75</v>
+      </c>
+      <c r="P53" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q53" s="5">
+        <v>831.5</v>
+      </c>
+      <c r="R53" s="5">
+        <v>415.75</v>
+      </c>
+      <c r="S53" s="5">
+        <v>3</v>
+      </c>
+      <c r="T53" s="5">
+        <v>1194</v>
+      </c>
+      <c r="U53" s="5">
+        <v>24.99</v>
+      </c>
+      <c r="V53" s="5">
+        <v>4228.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>